<commit_message>
Changed indicie direction to fix super high steady state temperature and added while loop
</commit_message>
<xml_diff>
--- a/Project 1 Results Template.xlsx
+++ b/Project 1 Results Template.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nordica\Google Drive\Oregon State\Teaching\ME 450\2021\Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Genevieve845\Desktop\Grad_school\Grad_School_classes\Applied_Heat_transfer\Projects\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3061F96F-83C1-4041-BA43-36C26F0D97A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9BBC87-BC67-437D-92BB-818B2D5F65AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24300" windowHeight="11955"/>
+    <workbookView xWindow="8385" yWindow="3060" windowWidth="15990" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -194,7 +203,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,12 +218,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407453"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -257,64 +272,60 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,24 +642,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1048651A-D361-40BA-BAF1-A2A72630FFC6}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="54.9296875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="55" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="true"/>
-    <col min="5" max="6" width="10.3984375" customWidth="true"/>
-    <col min="3" max="3" width="17" customWidth="true"/>
-    <col min="4" max="4" width="17" customWidth="true"/>
+    <col min="2" max="4" width="17" customWidth="1"/>
+    <col min="5" max="6" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -666,7 +675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -682,7 +691,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -700,7 +709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -718,7 +727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -736,17 +745,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="15" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="4"/>
@@ -754,69 +763,69 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="9">
-        <v>0.0006329113924050633</v>
+        <v>6.329113924050633E-4</v>
       </c>
       <c r="C9" s="9">
-        <v>0.0024793388429752063</v>
+        <v>2.4793388429752063E-3</v>
       </c>
       <c r="D9" s="9">
-        <v>0.14999999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="10">
-        <v>0.044999999999999998</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C10" s="10">
-        <v>0.044999999999999998</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D10" s="10">
-        <v>0.044999999999999998</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="10">
-        <v>0.00024677574987809589</v>
+        <v>2.4677574987809589E-4</v>
       </c>
       <c r="C11" s="10">
-        <v>0.00024672920674317044</v>
+        <v>2.4672920674317044E-4</v>
       </c>
       <c r="D11" s="10">
-        <v>0.00024306652730852438</v>
+        <v>2.4306652730852438E-4</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="10">
-        <v>0.0051446076218720788</v>
+        <v>5.1446076218720788E-3</v>
       </c>
       <c r="C12" s="10">
-        <v>0.028149510150765823</v>
+        <v>2.8149510150765823E-2</v>
       </c>
       <c r="D12" s="10">
         <v>1.2498189154371551</v>
@@ -826,7 +835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -844,7 +853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
@@ -862,7 +871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
@@ -880,7 +889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
@@ -898,7 +907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
@@ -916,17 +925,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="17">
         <v>4499.9999999999991</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="17">
         <v>4499.9999999999991</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="17">
         <v>4499.9999999999991</v>
       </c>
       <c r="E18" s="4"/>
@@ -934,17 +943,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="17">
         <v>463</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="17">
         <v>463</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="17">
         <v>463</v>
       </c>
       <c r="E19" s="4"/>
@@ -952,7 +961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
@@ -970,7 +979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>23</v>
       </c>
@@ -983,19 +992,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
     </row>
-    <row r="26" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
     </row>
-    <row r="27" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
     </row>

</xml_diff>

<commit_message>
flipped indices all the way, and changed dx to equal 0.001 like dy, also changed max counts
</commit_message>
<xml_diff>
--- a/Project 1 Results Template.xlsx
+++ b/Project 1 Results Template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,12 +10,12 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9BBC87-BC67-437D-92BB-818B2D5F65AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8385" yWindow="3060" windowWidth="15990" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8385" yWindow="3060" windowWidth="15990" windowHeight="12165"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>ME 450/550 Project #1 Results Template</t>
   </si>
@@ -218,7 +218,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407453"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -229,7 +229,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -279,53 +279,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,22 +658,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1048651A-D361-40BA-BAF1-A2A72630FFC6}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="17" customWidth="1"/>
-    <col min="5" max="6" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="true"/>
+    <col min="5" max="6" width="10.42578125" customWidth="true"/>
+    <col min="3" max="3" width="17" customWidth="true"/>
+    <col min="4" max="4" width="17" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -675,7 +693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -691,7 +709,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -709,7 +727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -727,7 +745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -745,17 +763,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="4"/>
@@ -763,69 +781,69 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="9">
-        <v>6.329113924050633E-4</v>
+        <v>0.0006329113924050633</v>
       </c>
       <c r="C9" s="9">
-        <v>2.4793388429752063E-3</v>
+        <v>0.0024793388429752063</v>
       </c>
       <c r="D9" s="9">
-        <v>0.15</v>
+        <v>0.14999999999999999</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="10">
-        <v>4.4999999999999998E-2</v>
+        <v>0.044999999999999998</v>
       </c>
       <c r="C10" s="10">
-        <v>4.4999999999999998E-2</v>
+        <v>0.044999999999999998</v>
       </c>
       <c r="D10" s="10">
-        <v>4.4999999999999998E-2</v>
+        <v>0.044999999999999998</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="10">
-        <v>2.4677574987809589E-4</v>
+        <v>0.00024677574987809589</v>
       </c>
       <c r="C11" s="10">
-        <v>2.4672920674317044E-4</v>
+        <v>0.00024672920674317044</v>
       </c>
       <c r="D11" s="10">
-        <v>2.4306652730852438E-4</v>
+        <v>0.00024306652730852438</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="10">
-        <v>5.1446076218720788E-3</v>
+        <v>0.0051446076218720788</v>
       </c>
       <c r="C12" s="10">
-        <v>2.8149510150765823E-2</v>
+        <v>0.028149510150765823</v>
       </c>
       <c r="D12" s="10">
         <v>1.2498189154371551</v>
@@ -835,7 +853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -853,7 +871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
@@ -871,7 +889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
@@ -889,7 +907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
@@ -907,7 +925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
@@ -925,7 +943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
@@ -943,7 +961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
@@ -961,7 +979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
@@ -979,7 +997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>23</v>
       </c>
@@ -992,19 +1010,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" x14ac:dyDescent="0.25">
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" x14ac:dyDescent="0.25">
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" x14ac:dyDescent="0.25">
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" x14ac:dyDescent="0.25">
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
     </row>

</xml_diff>

<commit_message>
added plots, fixed excel outputs
</commit_message>
<xml_diff>
--- a/Project 1 Results Template.xlsx
+++ b/Project 1 Results Template.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Genevieve845\Desktop\Grad_school\Grad_School_classes\Applied_Heat_transfer\Projects\Project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Austin\Documents\OSU\2020-2021\Winter 2021\ME 550\Project 1\HeatXfer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9BBC87-BC67-437D-92BB-818B2D5F65AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7FA3BE-7F46-4AF2-BBA4-A9BBA6D95270}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8385" yWindow="3060" windowWidth="15990" windowHeight="12165"/>
+    <workbookView xWindow="6036" yWindow="1284" windowWidth="23268" windowHeight="13848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>ME 450/550 Project #1 Results Template</t>
   </si>
@@ -203,7 +203,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,18 +218,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407453"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -279,69 +273,52 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,24 +635,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1048651A-D361-40BA-BAF1-A2A72630FFC6}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="55" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="55" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="true"/>
-    <col min="5" max="6" width="10.42578125" customWidth="true"/>
-    <col min="3" max="3" width="17" customWidth="true"/>
-    <col min="4" max="4" width="17" customWidth="true"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="6" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -693,7 +670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -709,7 +686,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -727,7 +704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -745,7 +722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -763,17 +740,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="16" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="4"/>
@@ -781,79 +758,79 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="9">
-        <v>0.0006329113924050633</v>
+        <v>6.329113924050633E-4</v>
       </c>
       <c r="C9" s="9">
-        <v>0.0024793388429752063</v>
+        <v>2.4793388429752063E-3</v>
       </c>
       <c r="D9" s="9">
-        <v>0.14999999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="10">
-        <v>0.044999999999999998</v>
+        <v>1E-3</v>
       </c>
       <c r="C10" s="10">
-        <v>0.044999999999999998</v>
+        <v>1E-3</v>
       </c>
       <c r="D10" s="10">
-        <v>0.044999999999999998</v>
+        <v>1E-3</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="10">
-        <v>0.00024677574987809589</v>
+        <v>0.24998417821656865</v>
       </c>
       <c r="C11" s="10">
-        <v>0.00024672920674317044</v>
+        <v>0.24993803189291913</v>
       </c>
       <c r="D11" s="10">
-        <v>0.00024306652730852438</v>
+        <v>0.24630541871921183</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="10">
-        <v>0.0051446076218720788</v>
+        <v>2.573577621669515E-3</v>
       </c>
       <c r="C12" s="10">
-        <v>0.028149510150765823</v>
+        <v>1.4081781376518221E-2</v>
       </c>
       <c r="D12" s="10">
-        <v>1.2498189154371551</v>
+        <v>0.62541871921182257</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -871,7 +848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
@@ -889,7 +866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
@@ -907,7 +884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
@@ -925,7 +902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
@@ -943,43 +920,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="29.4" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="17">
-        <v>4499.9999999999991</v>
-      </c>
-      <c r="C18" s="17">
-        <v>4499.9999999999991</v>
-      </c>
-      <c r="D18" s="17">
-        <v>4499.9999999999991</v>
+      <c r="B18" s="15">
+        <v>2553.6666666666665</v>
+      </c>
+      <c r="C18" s="15">
+        <v>2553.6666666666665</v>
+      </c>
+      <c r="D18" s="15">
+        <v>2553.6666666666665</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="19" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="17">
-        <v>463</v>
-      </c>
-      <c r="C19" s="17">
-        <v>463</v>
-      </c>
-      <c r="D19" s="17">
-        <v>463</v>
+      <c r="B19" s="15">
+        <v>126.98267125644384</v>
+      </c>
+      <c r="C19" s="15">
+        <v>126.98267125644384</v>
+      </c>
+      <c r="D19" s="15">
+        <v>126.98267125644384</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
@@ -997,7 +974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>23</v>
       </c>
@@ -1010,19 +987,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
     </row>
-    <row r="26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
     </row>
-    <row r="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
     </row>

</xml_diff>

<commit_message>
added LC to plots, fixed goal temp markers on plots, changed tolerance for steady state convergence to 1e-5, moved centerline temp plot into while loop and added if statements to plot only the slowest material at its half time to goal temp, added outputs for loop counts and temp array sizes to help with trouble shooting, added tic and toc to time loops -- AMW
</commit_message>
<xml_diff>
--- a/Project 1 Results Template.xlsx
+++ b/Project 1 Results Template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,12 +10,12 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7FA3BE-7F46-4AF2-BBA4-A9BBA6D95270}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6036" yWindow="1284" windowWidth="23268" windowHeight="13848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6036" yWindow="1284" windowWidth="23268" windowHeight="13848"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>ME 450/550 Project #1 Results Template</t>
   </si>
@@ -218,12 +218,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407453"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -273,52 +273,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,24 +675,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1048651A-D361-40BA-BAF1-A2A72630FFC6}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="6" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="true"/>
+    <col min="3" max="3" width="14.77734375" customWidth="true"/>
+    <col min="4" max="4" width="13.6640625" customWidth="true"/>
+    <col min="5" max="6" width="10.44140625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" ht="17.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -670,7 +710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -686,7 +726,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -704,7 +744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -722,7 +762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -740,17 +780,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="35" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="4"/>
@@ -758,43 +798,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="9">
-        <v>6.329113924050633E-4</v>
+        <v>0.0006329113924050633</v>
       </c>
       <c r="C9" s="9">
-        <v>2.4793388429752063E-3</v>
+        <v>0.0024793388429752063</v>
       </c>
       <c r="D9" s="9">
-        <v>0.15</v>
+        <v>0.14999999999999999</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="10">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="C10" s="10">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="D10" s="10">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -812,15 +852,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="10">
-        <v>2.573577621669515E-3</v>
+        <v>0.002573577621669515</v>
       </c>
       <c r="C12" s="10">
-        <v>1.4081781376518221E-2</v>
+        <v>0.014081781376518221</v>
       </c>
       <c r="D12" s="10">
         <v>0.62541871921182257</v>
@@ -830,7 +870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -848,7 +888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
@@ -866,7 +906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
@@ -884,7 +924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
@@ -902,7 +942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
@@ -920,7 +960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="29.4" x14ac:dyDescent="0.3">
+    <row r="18" ht="29.4" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
@@ -938,7 +978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="19" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
@@ -956,7 +996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
@@ -974,7 +1014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>23</v>
       </c>
@@ -987,19 +1027,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" x14ac:dyDescent="0.3">
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" x14ac:dyDescent="0.3">
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" x14ac:dyDescent="0.3">
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" x14ac:dyDescent="0.3">
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
     </row>

</xml_diff>

<commit_message>
found a mistake in the time step calc for the bottom corners, did not have an effect on the answer, but fixed the problem in the function file. -- AMW
</commit_message>
<xml_diff>
--- a/Project 1 Results Template.xlsx
+++ b/Project 1 Results Template.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>ME 450/550 Project #1 Results Template</t>
   </si>
@@ -223,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -293,11 +293,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
@@ -359,6 +363,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,13 +792,13 @@
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="39" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="4"/>

</xml_diff>